<commit_message>
J'ai réogarnisé les fichiers
</commit_message>
<xml_diff>
--- a/Cahier des charges technique.xlsx
+++ b/Cahier des charges technique.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baptiste\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baptiste\Documents\Epita\Chamourai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE111500-E323-471C-9A2A-98B010E97E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09907940-886F-4EE5-9CF1-7999345E99A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
   <si>
     <t>Nom du groupe :</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Assets</t>
   </si>
   <si>
-    <t xml:space="preserve">Codes/Programation </t>
-  </si>
-  <si>
     <t>Les Chatpitres</t>
   </si>
   <si>
@@ -313,15 +310,9 @@
     <t>Gameplay/Mécanique</t>
   </si>
   <si>
-    <t>Code/Programation</t>
-  </si>
-  <si>
     <t>Implémentation IA</t>
   </si>
   <si>
-    <t>Cinématique(s)</t>
-  </si>
-  <si>
     <t>loan.blanpain (R)</t>
   </si>
   <si>
@@ -341,9 +332,6 @@
   </si>
   <si>
     <t>lucas.huet (S)</t>
-  </si>
-  <si>
-    <t>loan.blanpain(S)</t>
   </si>
   <si>
     <t>baptiste.loiseau (S)</t>
@@ -571,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -623,6 +611,37 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -633,7 +652,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -658,45 +676,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -706,11 +700,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:E12"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1129,39 +1123,39 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1170,79 +1164,79 @@
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="41"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="38"/>
+      <c r="C6" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="29"/>
       <c r="E6" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="38"/>
+      <c r="C7" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="29"/>
       <c r="E7" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="38"/>
+      <c r="C8" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="29"/>
       <c r="E8" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -1253,135 +1247,135 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="A13" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
+      <c r="A27" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="40"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
@@ -1455,26 +1449,26 @@
       <c r="A32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="33"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="43"/>
     </row>
     <row r="33" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="37"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
@@ -1506,7 +1500,7 @@
       <c r="D36" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="25"/>
+      <c r="E36" s="35"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
@@ -1521,16 +1515,16 @@
       <c r="D37" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="26"/>
+      <c r="E37" s="36"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
     </row>
     <row r="39" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -1560,7 +1554,7 @@
       <c r="D40" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="22"/>
+      <c r="E40" s="33"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -1575,27 +1569,27 @@
       <c r="D41" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E41" s="22"/>
+      <c r="E41" s="33"/>
     </row>
     <row r="42" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
+      <c r="B42" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -1610,7 +1604,7 @@
       <c r="D44" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="22"/>
+      <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -1625,25 +1619,25 @@
       <c r="D45" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="22"/>
+      <c r="E45" s="33"/>
     </row>
     <row r="46" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
@@ -1661,40 +1655,28 @@
       <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
     </row>
     <row r="50" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
     </row>
     <row r="51" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
     <mergeCell ref="A51:E51"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E25"/>
@@ -1711,6 +1693,18 @@
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="B32:E32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1721,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1731,14 +1725,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1759,14 +1753,14 @@
       <c r="F2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="51" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" s="51" t="s">
-        <v>117</v>
+      <c r="H2" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
@@ -1774,16 +1768,16 @@
         <v>75</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>102</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3">
         <v>3</v>
@@ -1797,19 +1791,19 @@
     </row>
     <row r="4" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -1826,52 +1820,48 @@
         <v>76</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>77</v>
+      <c r="A6" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="50" t="s">
-        <v>88</v>
+      <c r="G6" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <v>4</v>
@@ -1882,10 +1872,10 @@
         <v>90</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>103</v>
+        <v>97</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1896,10 +1886,10 @@
         <v>91</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1910,10 +1900,10 @@
         <v>92</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1924,10 +1914,10 @@
         <v>93</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1935,28 +1925,19 @@
     </row>
     <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>103</v>
-      </c>
+    <row r="12" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2002,29 +1983,29 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="20" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="11" t="s">
         <v>71</v>
       </c>
@@ -2036,11 +2017,11 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="18">
         <v>0.6</v>
       </c>
@@ -2052,11 +2033,11 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
+      <c r="A22" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="17">
         <v>0</v>
       </c>
@@ -2068,11 +2049,11 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="49"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="18">
         <v>0.5</v>
       </c>
@@ -2084,27 +2065,19 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="E24" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="F24" s="18">
-        <v>1</v>
-      </c>
+      <c r="A24" s="49"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
+      <c r="A25" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="52"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="18">
         <v>0.5</v>
       </c>
@@ -2116,11 +2089,11 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
+      <c r="A26" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="18">
         <v>0</v>
       </c>
@@ -2132,11 +2105,11 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
+      <c r="A27" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="18">
         <v>0.4</v>
       </c>
@@ -2148,11 +2121,11 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="49"/>
+      <c r="A28" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="18">
         <v>0</v>
       </c>
@@ -2164,11 +2137,11 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="49"/>
+      <c r="A29" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="52"/>
+      <c r="C29" s="53"/>
       <c r="D29" s="18">
         <v>0.7</v>
       </c>
@@ -2180,11 +2153,11 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
+      <c r="A30" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="18">
         <v>0.25</v>
       </c>
@@ -2196,57 +2169,61 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
+      <c r="A32" s="48"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="46"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A19:F19"/>
@@ -2263,10 +2240,6 @@
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>